<commit_message>
#422 generates sequence of acts
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/TabularWorkflowBuilder.xlsx
+++ b/dsl/src/test/data/TabularWorkflowBuilder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E033074C-C39E-4793-9BA2-10245E107495}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6025C096-228B-4B5E-9FD1-3986B33167DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="3855" windowWidth="18900" windowHeight="10965" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
+    <workbookView xWindow="6675" yWindow="2175" windowWidth="15975" windowHeight="8340" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
   </bookViews>
   <sheets>
     <sheet name="TestItem_Workflow" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -115,10 +115,16 @@
     <t>class</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>property</t>
+  </si>
+  <si>
+    <t>activityVersion</t>
+  </si>
+  <si>
+    <t>SecondAgain</t>
+  </si>
+  <si>
+    <t>activityReference</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +192,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -251,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -261,6 +273,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -590,69 +604,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E00209-721C-400C-8B1A-B2E5C016AA01}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="9">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -683,17 +726,17 @@
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="10" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -774,17 +817,17 @@
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="10" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">

</xml_diff>

<commit_message>
#422 generates activity defs
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/TabularWorkflowBuilder.xlsx
+++ b/dsl/src/test/data/TabularWorkflowBuilder.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6025C096-228B-4B5E-9FD1-3986B33167DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A952972-1CEC-44FB-A141-68C7233CE6DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="2175" windowWidth="15975" windowHeight="8340" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="1" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
   </bookViews>
   <sheets>
     <sheet name="TestItem_Workflow" sheetId="1" r:id="rId1"/>
-    <sheet name="TestItem_First" sheetId="3" r:id="rId2"/>
-    <sheet name="TestItem_Second" sheetId="4" r:id="rId3"/>
+    <sheet name="TestItem_Activitites" sheetId="5" r:id="rId2"/>
+    <sheet name="TestItem_First" sheetId="3" r:id="rId3"/>
+    <sheet name="TestItem_Second" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -125,6 +126,57 @@
   </si>
   <si>
     <t>activityReference</t>
+  </si>
+  <si>
+    <t>Elementary</t>
+  </si>
+  <si>
+    <t>Composite</t>
+  </si>
+  <si>
+    <t>TestItem_Workflow</t>
+  </si>
+  <si>
+    <t>Loop</t>
+  </si>
+  <si>
+    <t>Dispensing</t>
+  </si>
+  <si>
+    <t>EndLoop</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>script</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>TestItem_SchemaFirst:0</t>
+  </si>
+  <si>
+    <t>TestItem_SchemaSecond:0</t>
+  </si>
+  <si>
+    <t>TestItem_ScriptSecond:0</t>
+  </si>
+  <si>
+    <t>TestItem_QueryFirst:0</t>
   </si>
 </sst>
 </file>
@@ -149,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,8 +250,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -259,11 +317,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -275,6 +362,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -285,6 +376,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -604,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E00209-721C-400C-8B1A-B2E5C016AA01}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,15 +717,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="12"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -691,6 +788,21 @@
         <v>28</v>
       </c>
       <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -703,11 +815,140 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF65472-52CB-4998-8893-FEF6E36CE646}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C766949-E7B6-4270-B058-3321C5ED677A}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,17 +967,17 @@
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="12" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -793,12 +1034,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BACA9192-27E2-4595-A6A1-907E3615407F}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,17 +1058,17 @@
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="12" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">

</xml_diff>

<commit_message>
Add spearate tests and excel for Loop development #422
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/TabularWorkflowBuilder.xlsx
+++ b/dsl/src/test/data/TabularWorkflowBuilder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB91EF1-E720-4775-9310-C21ACCE91401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40E5B53-45F2-4FA1-A418-0D8D4CDCA4F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="3040" windowWidth="19200" windowHeight="10160" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16800" windowHeight="10155" activeTab="1" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
   </bookViews>
   <sheets>
     <sheet name="TestItem_Sequence" sheetId="1" r:id="rId1"/>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E00209-721C-400C-8B1A-B2E5C016AA01}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -736,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB994CB5-5202-4AA9-9615-3F210D52ADE5}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>